<commit_message>
Menu Test Cases added
</commit_message>
<xml_diff>
--- a/RegressionTests/src/test/java/testData/testData.xlsx
+++ b/RegressionTests/src/test/java/testData/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -44,6 +44,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>WrongPassLogin</t>
+  </si>
+  <si>
+    <t>OpenContactPage</t>
+  </si>
+  <si>
+    <t>OpenSalesPage</t>
+  </si>
+  <si>
+    <t>OpenPurchasePage</t>
+  </si>
+  <si>
+    <t>OpenHomePage</t>
   </si>
 </sst>
 </file>
@@ -390,15 +405,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
@@ -447,6 +462,52 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>